<commit_message>
Adicionando caminho da pasta dados
</commit_message>
<xml_diff>
--- a/dados/EstatisticasDosJogadores.xlsx
+++ b/dados/EstatisticasDosJogadores.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:E108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,10 +472,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E2" t="n">
         <v>3</v>
@@ -514,7 +514,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" t="n">
         <v>4</v>
@@ -524,35 +524,37 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Reinaldo</t>
+          <t>Yuri Alberto</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Mirassol</t>
+          <t>Corinthians</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5" t="n">
         <v>4</v>
       </c>
-      <c r="E5" t="inlineStr"/>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Pedro</t>
+          <t>Kaio Jorge</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Flamengo</t>
+          <t>Cruzeiro</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D6" t="n">
         <v>4</v>
@@ -564,54 +566,52 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Memphis Depay</t>
+          <t>Reinaldo</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Corinthians</t>
+          <t>Mirassol</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
-      </c>
-      <c r="E7" t="n">
-        <v>1</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Ferreira</t>
+          <t>Pedro</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>Flamengo</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Kaio Jorge</t>
+          <t>Memphis Depay</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Cruzeiro</t>
+          <t>Corinthians</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -621,41 +621,43 @@
         <v>3</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Rony</t>
+          <t>Ferreira</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Atlético Mineiro</t>
+          <t>São Paulo</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E10" t="n">
         <v>2</v>
       </c>
-      <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Gabriel Taliari</t>
+          <t>Gabriel Barbosa</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Juventude</t>
+          <t>Cruzeiro</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D11" t="n">
         <v>2</v>
@@ -665,16 +667,16 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Álvaro Barreal</t>
+          <t>Rony</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Santos</t>
+          <t>Atlético Mineiro</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D12" t="n">
         <v>2</v>
@@ -684,16 +686,16 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Ignacio Laquintana</t>
+          <t>Gabriel Taliari</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Bragantino</t>
+          <t>Juventude</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D13" t="n">
         <v>2</v>
@@ -703,54 +705,50 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Igor Jesus</t>
+          <t>Álvaro Barreal</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Botafogo</t>
+          <t>Santos</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" t="n">
         <v>2</v>
       </c>
-      <c r="E14" t="n">
-        <v>1</v>
-      </c>
+      <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Alan Patrick</t>
+          <t>Marllon</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Internacional</t>
+          <t>Ceará</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D15" t="n">
         <v>2</v>
       </c>
-      <c r="E15" t="n">
-        <v>3</v>
-      </c>
+      <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Rafael Borré</t>
+          <t>Ignacio Laquintana</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Internacional</t>
+          <t>Bragantino</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -764,31 +762,33 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>José Manuel López</t>
+          <t>Igor Jesus</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Palmeiras</t>
+          <t>Botafogo</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D17" t="n">
         <v>2</v>
       </c>
-      <c r="E17" t="inlineStr"/>
+      <c r="E17" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Joaquín Piquerez</t>
+          <t>Alan Patrick</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Palmeiras</t>
+          <t>Internacional</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -797,17 +797,19 @@
       <c r="D18" t="n">
         <v>2</v>
       </c>
-      <c r="E18" t="inlineStr"/>
+      <c r="E18" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Eduardo Sasha</t>
+          <t>Rafael Borré</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Bragantino</t>
+          <t>Internacional</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -816,23 +818,21 @@
       <c r="D19" t="n">
         <v>2</v>
       </c>
-      <c r="E19" t="n">
-        <v>1</v>
-      </c>
+      <c r="E19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Matheuzinho</t>
+          <t>José Manuel López</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Vitória</t>
+          <t>Palmeiras</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D20" t="n">
         <v>2</v>
@@ -842,33 +842,31 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Jefferson Savarino</t>
+          <t>Joaquín Piquerez</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Botafogo</t>
+          <t>Palmeiras</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D21" t="n">
         <v>2</v>
       </c>
-      <c r="E21" t="n">
-        <v>1</v>
-      </c>
+      <c r="E21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>André Silva</t>
+          <t>Eduardo Sasha</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>Bragantino</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -884,12 +882,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Daniel Borges</t>
+          <t>Matheuzinho</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Mirassol</t>
+          <t>Vitória</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -903,12 +901,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Facundo Torres Pérez</t>
+          <t>Jefferson Savarino</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Palmeiras</t>
+          <t>Botafogo</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -924,16 +922,16 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Enmerson Batalla</t>
+          <t>André Silva</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Juventude</t>
+          <t>São Paulo</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D25" t="n">
         <v>2</v>
@@ -945,16 +943,16 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Victor Gabriel</t>
+          <t>Daniel Borges</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Internacional</t>
+          <t>Mirassol</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D26" t="n">
         <v>2</v>
@@ -964,71 +962,73 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Dudu</t>
+          <t>Facundo Torres Pérez</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Cruzeiro</t>
+          <t>Palmeiras</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D27" t="n">
-        <v>1</v>
-      </c>
-      <c r="E27" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Gabriel Barbosa</t>
+          <t>Enmerson Batalla</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Cruzeiro</t>
+          <t>Juventude</t>
         </is>
       </c>
       <c r="C28" t="n">
         <v>6</v>
       </c>
       <c r="D28" t="n">
-        <v>1</v>
-      </c>
-      <c r="E28" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="E28" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Lucas Ramon</t>
+          <t>Victor Gabriel</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Mirassol</t>
+          <t>Internacional</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D29" t="n">
-        <v>1</v>
-      </c>
-      <c r="E29" t="n">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Matías Arezo</t>
+          <t>Dudu</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Grêmio</t>
+          <t>Cruzeiro</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -1037,19 +1037,17 @@
       <c r="D30" t="n">
         <v>1</v>
       </c>
-      <c r="E30" t="n">
-        <v>1</v>
-      </c>
+      <c r="E30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Edenilson</t>
+          <t>Lucas Ramon</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Grêmio</t>
+          <t>Mirassol</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -1058,17 +1056,19 @@
       <c r="D31" t="n">
         <v>1</v>
       </c>
-      <c r="E31" t="inlineStr"/>
+      <c r="E31" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Juan Lucero</t>
+          <t>Matías Arezo</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Fortaleza</t>
+          <t>Grêmio</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -1077,21 +1077,23 @@
       <c r="D32" t="n">
         <v>1</v>
       </c>
-      <c r="E32" t="inlineStr"/>
+      <c r="E32" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Tinga</t>
+          <t>Edenilson</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Fortaleza</t>
+          <t>Grêmio</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D33" t="n">
         <v>1</v>
@@ -1101,16 +1103,16 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Bruno Henrique</t>
+          <t>Juan Lucero</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Internacional</t>
+          <t>Fortaleza</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D34" t="n">
         <v>1</v>
@@ -1120,16 +1122,16 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Léo Pereira</t>
+          <t>Tinga</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Flamengo</t>
+          <t>Fortaleza</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D35" t="n">
         <v>1</v>
@@ -1139,12 +1141,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Nuno Moreira</t>
+          <t>Bruno Henrique</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Vasco da Gama</t>
+          <t>Internacional</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -1153,23 +1155,21 @@
       <c r="D36" t="n">
         <v>1</v>
       </c>
-      <c r="E36" t="n">
-        <v>1</v>
-      </c>
+      <c r="E36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Gilberto</t>
+          <t>Léo Pereira</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Bahia</t>
+          <t>Flamengo</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D37" t="n">
         <v>1</v>
@@ -1179,31 +1179,33 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Héctor Hernández</t>
+          <t>Nuno Moreira</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Corinthians</t>
+          <t>Vasco da Gama</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D38" t="n">
         <v>1</v>
       </c>
-      <c r="E38" t="inlineStr"/>
+      <c r="E38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Marllon</t>
+          <t>Gilberto</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Ceará</t>
+          <t>Bahia</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -1217,16 +1219,16 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Eric Ramires</t>
+          <t>Héctor Hernández</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Bragantino</t>
+          <t>Corinthians</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D40" t="n">
         <v>1</v>
@@ -1236,12 +1238,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Yuri Alberto</t>
+          <t>Eric Ramires</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Corinthians</t>
+          <t>Bragantino</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -1250,9 +1252,7 @@
       <c r="D41" t="n">
         <v>1</v>
       </c>
-      <c r="E41" t="n">
-        <v>1</v>
-      </c>
+      <c r="E41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1266,7 +1266,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D42" t="n">
         <v>1</v>
@@ -1287,7 +1287,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D43" t="n">
         <v>1</v>
@@ -1306,7 +1306,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D44" t="n">
         <v>1</v>
@@ -1344,7 +1344,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D46" t="n">
         <v>1</v>
@@ -1363,7 +1363,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D47" t="n">
         <v>1</v>
@@ -1403,7 +1403,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D49" t="n">
         <v>1</v>
@@ -1422,7 +1422,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D50" t="n">
         <v>1</v>
@@ -1441,7 +1441,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D51" t="n">
         <v>1</v>
@@ -1460,7 +1460,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D52" t="n">
         <v>1</v>
@@ -1479,7 +1479,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D53" t="n">
         <v>1</v>
@@ -1498,7 +1498,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D54" t="n">
         <v>1</v>
@@ -1517,7 +1517,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D55" t="n">
         <v>1</v>
@@ -1536,7 +1536,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D56" t="n">
         <v>1</v>
@@ -1614,7 +1614,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D60" t="n">
         <v>1</v>
@@ -1633,7 +1633,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D61" t="n">
         <v>1</v>
@@ -1673,12 +1673,14 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D63" t="n">
         <v>1</v>
       </c>
-      <c r="E63" t="inlineStr"/>
+      <c r="E63" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1692,7 +1694,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D64" t="n">
         <v>1</v>
@@ -1711,7 +1713,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D65" t="n">
         <v>1</v>
@@ -1768,7 +1770,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D68" t="n">
         <v>1</v>
@@ -1806,7 +1808,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D70" t="n">
         <v>1</v>
@@ -1825,13 +1827,13 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D71" t="n">
         <v>1</v>
       </c>
       <c r="E71" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72">
@@ -1846,7 +1848,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D72" t="n">
         <v>1</v>
@@ -1884,7 +1886,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D74" t="n">
         <v>1</v>
@@ -1903,7 +1905,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D75" t="n">
         <v>1</v>
@@ -1922,7 +1924,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D76" t="n">
         <v>1</v>
@@ -1960,7 +1962,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D78" t="n">
         <v>1</v>
@@ -2040,7 +2042,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D82" t="n">
         <v>1</v>
@@ -2099,7 +2101,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D85" t="n">
         <v>1</v>
@@ -2118,7 +2120,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D86" t="n">
         <v>1</v>
@@ -2158,7 +2160,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D88" t="n">
         <v>1</v>
@@ -2219,7 +2221,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D91" t="n">
         <v>1</v>
@@ -2238,7 +2240,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D92" t="n">
         <v>1</v>
@@ -2257,7 +2259,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D93" t="n">
         <v>1</v>
@@ -2276,7 +2278,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D94" t="n">
         <v>1</v>
@@ -2297,7 +2299,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D95" t="n">
         <v>1</v>
@@ -2316,7 +2318,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D96" t="n">
         <v>1</v>
@@ -2337,7 +2339,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D97" t="n">
         <v>1</v>
@@ -2356,7 +2358,7 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D98" t="n">
         <v>1</v>
@@ -2375,12 +2377,185 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D99" t="n">
         <v>1</v>
       </c>
       <c r="E99" t="inlineStr"/>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Pablo Felipe</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Sport</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>4</v>
+      </c>
+      <c r="D100" t="n">
+        <v>1</v>
+      </c>
+      <c r="E100" t="inlineStr"/>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Kevin Serna</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Fluminense</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>7</v>
+      </c>
+      <c r="D101" t="n">
+        <v>1</v>
+      </c>
+      <c r="E101" t="inlineStr"/>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Everaldo</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Fluminense</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>7</v>
+      </c>
+      <c r="D102" t="n">
+        <v>1</v>
+      </c>
+      <c r="E102" t="inlineStr"/>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Braian Aguirre</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Internacional</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>7</v>
+      </c>
+      <c r="D103" t="n">
+        <v>1</v>
+      </c>
+      <c r="E103" t="inlineStr"/>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Thiago Maia</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Internacional</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>7</v>
+      </c>
+      <c r="D104" t="n">
+        <v>1</v>
+      </c>
+      <c r="E104" t="inlineStr"/>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Igor Coronado</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Corinthians</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>4</v>
+      </c>
+      <c r="D105" t="n">
+        <v>1</v>
+      </c>
+      <c r="E105" t="inlineStr"/>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Cauly</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Bahia</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
+        <v>7</v>
+      </c>
+      <c r="D106" t="n">
+        <v>1</v>
+      </c>
+      <c r="E106" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Vítor Roque</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Palmeiras</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>7</v>
+      </c>
+      <c r="D107" t="n">
+        <v>1</v>
+      </c>
+      <c r="E107" t="inlineStr"/>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Cristian Olivera</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Grêmio</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>4</v>
+      </c>
+      <c r="D108" t="n">
+        <v>1</v>
+      </c>
+      <c r="E108" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>